<commit_message>
Add E spigot test, some debugging of asm/emu
</commit_message>
<xml_diff>
--- a/argus400/doc/Argus400.xlsx
+++ b/argus400/doc/Argus400.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richarde/Library/Mobile Documents/com~apple~CloudDocs/Documents/Development/git/ferranti-argus/argus400/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00928D3F-AA97-9949-BD8E-2A589ECFD0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435086D3-C4A5-5D41-A6D2-28E89D202735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="127">
   <si>
     <t>Opcode</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>Source of Zeroes (and Acc 0)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -669,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -718,6 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +942,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1291,10 +1295,10 @@
         <v>30</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>31</v>
@@ -1324,10 +1328,10 @@
         <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>33</v>
@@ -1357,10 +1361,10 @@
         <v>34</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>35</v>
@@ -1390,10 +1394,10 @@
         <v>36</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>37</v>
@@ -1686,7 +1690,9 @@
       <c r="D23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="36" t="s">
+        <v>126</v>
+      </c>
       <c r="F23" s="6" t="s">
         <v>10</v>
       </c>
@@ -1783,10 +1789,12 @@
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="6"/>
+      <c r="E26" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="G26" s="6" t="s">
         <v>61</v>
       </c>
@@ -2367,7 +2375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F2A982-FB44-FB42-82D9-F855B50E2A0E}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix all sto type syntax
</commit_message>
<xml_diff>
--- a/argus400/doc/Argus400.xlsx
+++ b/argus400/doc/Argus400.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richarde/Library/Mobile Documents/com~apple~CloudDocs/Documents/Development/git/ferranti-argus/argus400/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435086D3-C4A5-5D41-A6D2-28E89D202735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B448E657-220C-AE4E-BB1A-D8876D6206A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
@@ -379,9 +379,6 @@
     <t>Use the register's location in the memory map and the MSUB instruction</t>
   </si>
   <si>
-    <t>MSUB &lt;reg&gt;, 0</t>
-  </si>
-  <si>
     <t>The assembler will correctly use the register's memory map location as the address operand in this case</t>
   </si>
   <si>
@@ -416,6 +413,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>MSUB 0, &lt;reg address&gt;</t>
   </si>
 </sst>
 </file>
@@ -713,6 +713,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -721,7 +722,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -942,7 +942,7 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -997,7 +997,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>96</v>
@@ -1690,8 +1690,8 @@
       <c r="D23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="36" t="s">
-        <v>126</v>
+      <c r="E23" s="32" t="s">
+        <v>125</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>10</v>
@@ -1724,7 +1724,7 @@
         <v>56</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>10</v>
@@ -1789,8 +1789,8 @@
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="36" t="s">
-        <v>126</v>
+      <c r="E26" s="32" t="s">
+        <v>125</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>10</v>
@@ -2072,14 +2072,14 @@
       <c r="A37" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
+      <c r="B37" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2100,10 +2100,10 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2157,7 +2157,7 @@
         <v>00000</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -2221,7 +2221,7 @@
         <f>DEC2OCT(5,5)</f>
         <v>00005</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="35" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       <c r="B9" s="19">
         <v>7777</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="36"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="str">
@@ -2255,7 +2255,7 @@
       <c r="B11" s="17">
         <v>10001</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="35" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       <c r="B12" s="19">
         <v>10007</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="str">
@@ -2375,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F2A982-FB44-FB42-82D9-F855B50E2A0E}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2428,12 +2428,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B12" s="12" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
@@ -2441,22 +2441,22 @@
         <v>3</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>